<commit_message>
Update Commandes Budjet Juin
</commit_message>
<xml_diff>
--- a/GestionDeProjet/Commandes/Commande_n_3.xlsx
+++ b/GestionDeProjet/Commandes/Commande_n_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robot_Surveillance_V3\GestionDeProjet\Commandes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECEF8B3-C204-49C5-95A7-2FA2C5F52000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44E5479-A32C-42E1-976A-5E4123F95ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commande_3" sheetId="1" r:id="rId1"/>
@@ -492,14 +492,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -786,7 +786,7 @@
   <dimension ref="A1:I974"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +857,7 @@
         <f>D3*E3</f>
         <v>16.059999999999999</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="43" t="s">
         <v>17</v>
       </c>
     </row>
@@ -877,9 +877,7 @@
       <c r="E4" s="9">
         <v>2</v>
       </c>
-      <c r="F4" s="34">
-        <v>20</v>
-      </c>
+      <c r="F4" s="34"/>
       <c r="G4" s="24">
         <f t="shared" ref="G4" si="0">D4*E4</f>
         <v>29.68</v>
@@ -956,7 +954,7 @@
       </c>
       <c r="F8" s="28">
         <f>SUM(F3:F4)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G8" s="25">
         <f>SUM(G3:G7)</f>
@@ -983,7 +981,7 @@
       </c>
       <c r="F11" s="16">
         <f>F8+G8</f>
-        <v>104.52999999999999</v>
+        <v>84.529999999999987</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -5329,7 +5327,7 @@
       <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43">
+      <c r="A3" s="44">
         <v>2</v>
       </c>
       <c r="B3" s="11"/>
@@ -5356,7 +5354,7 @@
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
         <v>19</v>

</xml_diff>